<commit_message>
Some technical stuff james, marie and matt fixed testing page
</commit_message>
<xml_diff>
--- a/CO600 Folder imported from Google Drive/Testing/Full Testing.xlsx
+++ b/CO600 Folder imported from Google Drive/Testing/Full Testing.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\public_html\CO600 Folder imported from Google Drive\Testing\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="163">
   <si>
     <t>version 1.5.2</t>
   </si>
@@ -491,23 +499,33 @@
   </si>
   <si>
     <t>it should show the information about the booking you have made recently aswell as the other bookings you have made</t>
+  </si>
+  <si>
+    <t>is the search box working</t>
+  </si>
+  <si>
+    <t>Does the search box prevent XSS attacks</t>
+  </si>
+  <si>
+    <t>Does the search box prevent SQL injections?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -517,7 +535,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -532,6 +550,7 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -546,59 +565,50 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <font/>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
+          <fgColor rgb="FF980000"/>
+          <bgColor rgb="FF980000"/>
         </patternFill>
       </fill>
-      <alignment/>
       <border>
         <left/>
         <right/>
@@ -607,14 +617,12 @@
       </border>
     </dxf>
     <dxf>
-      <font/>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFA61C00"/>
           <bgColor rgb="FFA61C00"/>
         </patternFill>
       </fill>
-      <alignment/>
       <border>
         <left/>
         <right/>
@@ -623,14 +631,12 @@
       </border>
     </dxf>
     <dxf>
-      <font/>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF980000"/>
-          <bgColor rgb="FF980000"/>
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
         </patternFill>
       </fill>
-      <alignment/>
       <border>
         <left/>
         <right/>
@@ -639,28 +645,297 @@
       </border>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:J76"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="24.0"/>
-    <col customWidth="1" min="3" max="3" width="21.14"/>
-    <col customWidth="1" min="4" max="4" width="21.57"/>
-    <col customWidth="1" min="5" max="5" width="6.0"/>
-    <col customWidth="1" min="8" max="8" width="21.29"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="6" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -671,7 +946,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4">
+    <row r="3" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -697,9 +973,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>11</v>
@@ -726,9 +1002,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>17</v>
@@ -752,9 +1028,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>19</v>
@@ -778,9 +1054,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>22</v>
@@ -794,7 +1070,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
@@ -820,7 +1096,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>26</v>
       </c>
@@ -846,7 +1122,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>29</v>
       </c>
@@ -872,7 +1148,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>32</v>
       </c>
@@ -898,7 +1174,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>35</v>
       </c>
@@ -924,7 +1200,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>37</v>
       </c>
@@ -950,7 +1226,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>39</v>
       </c>
@@ -976,7 +1252,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>42</v>
       </c>
@@ -1002,7 +1278,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>45</v>
       </c>
@@ -1028,7 +1304,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>48</v>
       </c>
@@ -1054,7 +1330,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>51</v>
       </c>
@@ -1080,9 +1356,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>54</v>
@@ -1106,9 +1382,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>56</v>
@@ -1132,9 +1408,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>58</v>
@@ -1158,9 +1434,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>61</v>
@@ -1184,9 +1460,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>64</v>
@@ -1210,9 +1486,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>64</v>
@@ -1236,9 +1512,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>71</v>
@@ -1262,9 +1538,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>71</v>
@@ -1288,9 +1564,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>77</v>
@@ -1314,9 +1590,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>77</v>
@@ -1340,7 +1616,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
@@ -1348,21 +1624,21 @@
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>83</v>
@@ -1386,9 +1662,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>83</v>
@@ -1412,9 +1688,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>83</v>
@@ -1438,9 +1714,9 @@
         <v>88</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>89</v>
@@ -1464,9 +1740,9 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>94</v>
@@ -1490,9 +1766,9 @@
         <v>97</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>98</v>
@@ -1516,9 +1792,9 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:8" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>101</v>
@@ -1542,9 +1818,9 @@
         <v>105</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>101</v>
@@ -1568,9 +1844,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>101</v>
@@ -1594,7 +1870,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="10"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
@@ -1604,14 +1880,14 @@
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
     </row>
-    <row r="44">
+    <row r="44" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>111</v>
@@ -1635,9 +1911,9 @@
         <v>114</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>111</v>
@@ -1661,9 +1937,9 @@
         <v>119</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>111</v>
@@ -1687,9 +1963,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>121</v>
@@ -1713,9 +1989,9 @@
         <v>125</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>126</v>
@@ -1739,12 +2015,12 @@
         <v>129</v>
       </c>
       <c r="I49" s="11">
-        <v>42754.0</v>
-      </c>
-    </row>
-    <row r="50">
+        <v>42754</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>130</v>
@@ -1768,9 +2044,9 @@
         <v>129</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>131</v>
@@ -1794,9 +2070,9 @@
         <v>129</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>132</v>
@@ -1820,9 +2096,9 @@
         <v>129</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>133</v>
@@ -1846,9 +2122,9 @@
         <v>129</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>130</v>
@@ -1872,9 +2148,9 @@
         <v>129</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>134</v>
@@ -1898,9 +2174,9 @@
         <v>138</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>134</v>
@@ -1924,9 +2200,9 @@
         <v>129</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>140</v>
@@ -1938,9 +2214,9 @@
       <c r="G57" s="6"/>
       <c r="H57" s="6"/>
     </row>
-    <row r="58">
+    <row r="58" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>141</v>
@@ -1952,9 +2228,9 @@
       <c r="G58" s="6"/>
       <c r="H58" s="6"/>
     </row>
-    <row r="59">
+    <row r="59" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>142</v>
@@ -1966,9 +2242,9 @@
       <c r="G59" s="6"/>
       <c r="H59" s="6"/>
     </row>
-    <row r="60">
+    <row r="60" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>143</v>
@@ -1980,9 +2256,9 @@
       <c r="G60" s="6"/>
       <c r="H60" s="6"/>
     </row>
-    <row r="61">
+    <row r="61" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>144</v>
@@ -1994,9 +2270,9 @@
       <c r="G61" s="6"/>
       <c r="H61" s="6"/>
     </row>
-    <row r="62">
+    <row r="62" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>145</v>
@@ -2008,9 +2284,9 @@
       <c r="G62" s="6"/>
       <c r="H62" s="6"/>
     </row>
-    <row r="63">
+    <row r="63" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>146</v>
@@ -2022,9 +2298,9 @@
       <c r="G63" s="6"/>
       <c r="H63" s="6"/>
     </row>
-    <row r="64">
+    <row r="64" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>147</v>
@@ -2036,9 +2312,9 @@
       <c r="G64" s="6"/>
       <c r="H64" s="6"/>
     </row>
-    <row r="65">
+    <row r="65" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A65" s="4">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>148</v>
@@ -2050,9 +2326,9 @@
       <c r="G65" s="6"/>
       <c r="H65" s="6"/>
     </row>
-    <row r="66">
+    <row r="66" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
-        <v>44.0</v>
+        <v>44</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>149</v>
@@ -2064,9 +2340,9 @@
       <c r="G66" s="6"/>
       <c r="H66" s="6"/>
     </row>
-    <row r="67">
+    <row r="67" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>150</v>
@@ -2090,9 +2366,9 @@
         <v>154</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>150</v>
@@ -2116,9 +2392,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
-        <v>47.0</v>
+        <v>47</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>156</v>
@@ -2132,9 +2408,9 @@
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
     </row>
-    <row r="70">
+    <row r="70" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>158</v>
@@ -2148,9 +2424,13 @@
       <c r="G70" s="6"/>
       <c r="H70" s="6"/>
     </row>
-    <row r="71">
-      <c r="A71" s="6"/>
-      <c r="B71" s="6"/>
+    <row r="71" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A71" s="6">
+        <v>49</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>160</v>
+      </c>
       <c r="C71" s="6"/>
       <c r="D71" s="6"/>
       <c r="E71" s="6"/>
@@ -2158,9 +2438,79 @@
       <c r="G71" s="6"/>
       <c r="H71" s="6"/>
     </row>
+    <row r="72" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="6">
+        <v>50</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+    </row>
+    <row r="73" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A73" s="6">
+        <v>51</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+    </row>
+    <row r="74" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="6">
+        <v>52</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+    </row>
+    <row r="75" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="6">
+        <v>53</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+    </row>
+    <row r="76" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="6">
+        <v>54</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="L9">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="1">
       <formula>LEN(TRIM(L9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2170,10 +2520,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1000">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH(("Y"),(F1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cleaned up older files
</commit_message>
<xml_diff>
--- a/CO600 Folder imported from Google Drive/Testing/Full Testing.xlsx
+++ b/CO600 Folder imported from Google Drive/Testing/Full Testing.xlsx
@@ -19,16 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="163">
-  <si>
-    <t>version 1.5.2</t>
-  </si>
-  <si>
-    <t>version 1.5.3</t>
-  </si>
-  <si>
-    <t>version 1.5.4</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="300">
   <si>
     <t>Test Number</t>
   </si>
@@ -69,9 +60,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>I would like to point out that our site does not work on IE, LOL who uses that anyway</t>
-  </si>
-  <si>
     <t>Index page loads first?</t>
   </si>
   <si>
@@ -351,9 +339,6 @@
     <t>same as above</t>
   </si>
   <si>
-    <t>1.6.01</t>
-  </si>
-  <si>
     <t>putting the agree form into the the php, this should show the agree form when it gets called rather than displayig it on a button click</t>
   </si>
   <si>
@@ -508,6 +493,432 @@
   </si>
   <si>
     <t>Does the search box prevent SQL injections?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">does the search box return the correct results </t>
+  </si>
+  <si>
+    <t xml:space="preserve">if I search for an item by name it should show me the items that have the same or simuilar  name </t>
+  </si>
+  <si>
+    <t>it shows me the correct results, BUT it only checks against the first name of the item meaning that some items might not show</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Look into a way where we check against the entire string of charactors within the items name </t>
+  </si>
+  <si>
+    <t>does the search box work automatically</t>
+  </si>
+  <si>
+    <t xml:space="preserve">when typying it should automatically start searching the database for that item and displaying it </t>
+  </si>
+  <si>
+    <t xml:space="preserve">although it does work as intended, you can fine tune the results when you press return on the keyboard </t>
+  </si>
+  <si>
+    <t>look into a way where it can fine tune the results automatically without the use manually having to do it themseves</t>
+  </si>
+  <si>
+    <t>Does Item Filtering work:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">when selecting the item from the drop down box it should only show my items that have the same type as the ones choosen </t>
+  </si>
+  <si>
+    <t>EEG Headset filtering</t>
+  </si>
+  <si>
+    <t>when I select EEG headset from the filter list it should only show me EEG headsets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this worked correctly </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Book Filtering </t>
+  </si>
+  <si>
+    <t>when selecting Books from the Filter list it should only show me books</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lego Filtering </t>
+  </si>
+  <si>
+    <t xml:space="preserve">When selecting Lego it should only show me lego on the page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pi Filtering </t>
+  </si>
+  <si>
+    <t>when selecting PI it should only show me PI's</t>
+  </si>
+  <si>
+    <t>Filering an item and then searching</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if I filter an item and then search for an item it should only only search for items with same type as the type selected </t>
+  </si>
+  <si>
+    <t>this did not work, this is because the search box returns new results that are not covered by the filtering meaning that it avoids the prevouis filter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This can be fixed with some PHP and SQL changes, the SQL Will need to be chnaged based on the filter selection meaning that we should also send the result of the filter to the PHP where it returns the result from the search, the PHP will also need an if statement, because if the filter is set to all items the SQL database does not have an item for all Items so, if filter is set to all items it shoulld run the the normal SQL selection but if the Filter has been set to books for example it should run an sql with a WHERE clause meaning that it would only run the search based on the type selected </t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>does reszinig the my bookings page display the page in an easy to read format for phones</t>
+  </si>
+  <si>
+    <t>when I rezize the page it should fit for phone devices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it worked, although if you rezised the page back and then go to another page it goes back ot the bookings page which is bug </t>
+  </si>
+  <si>
+    <t>This could be fixed by removing the code that changes the page to fit on phones if the page is reloaded, or I could load both onto the page and then hide and display the other, this might be an easy fix</t>
+  </si>
+  <si>
+    <t>when I press the catalog button it should take me to the page with all the items</t>
+  </si>
+  <si>
+    <t>to make navagation easier the navagation was changed so that there is only one catalogue link which the user can press, this page will display all of the items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I should be able to click on an item and it should load information about that item to me </t>
+  </si>
+  <si>
+    <t>it works correctly</t>
+  </si>
+  <si>
+    <t>when im on an items page it should show me the correct information about that item</t>
+  </si>
+  <si>
+    <t>there should be a selection box with dates to book items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">todays current date should not appear in the list of days </t>
+  </si>
+  <si>
+    <t>there should be another selection box on the page, this should allow me to select how many days I would like to book the item forq</t>
+  </si>
+  <si>
+    <t>it works correclty</t>
+  </si>
+  <si>
+    <t>booking an item that im allowed to book, should send me an email saying which item I have booked, the person I have booked it from, they day I have choose to book it for and the day I should return the item</t>
+  </si>
+  <si>
+    <t>when I book an item it should tell me how many books I have</t>
+  </si>
+  <si>
+    <t>it works correcly, although I have to refresh the page to get it to update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">find a way to update the variable on the page </t>
+  </si>
+  <si>
+    <t>The variable is not being updated</t>
+  </si>
+  <si>
+    <t>when I book an item it should add it to the booking database</t>
+  </si>
+  <si>
+    <t>this works correctly allough if you want to book it for one day it should allow me to do that</t>
+  </si>
+  <si>
+    <t>when adding the days together it should -1 to allow to count the day that its being booked for</t>
+  </si>
+  <si>
+    <t>the code does not count the day you pick it up as a day that it is being booked for</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can I Book an item that has already been booked on the days choosen </t>
+  </si>
+  <si>
+    <t>can I book an item that has not been booked on the days chosen</t>
+  </si>
+  <si>
+    <t>can I Edit the User inline without the box appearing on the page</t>
+  </si>
+  <si>
+    <t>can I Edit the User inline without the box appearing on the page on Manage users page</t>
+  </si>
+  <si>
+    <t>when the admin wants to edit a users information they should be able to change one thing at a time if they should</t>
+  </si>
+  <si>
+    <t>this does not work, for example if the user wants to edit just a users name, then they would have to reset all of the other information to the same thing they already was</t>
+  </si>
+  <si>
+    <t>although it did not work as intended it still worked</t>
+  </si>
+  <si>
+    <t>this now works, the user can edit one thing at a time withought having to refil the same information</t>
+  </si>
+  <si>
+    <t>Can I edit the users UserType</t>
+  </si>
+  <si>
+    <t>Can I Edit the users Year</t>
+  </si>
+  <si>
+    <t>Can I edit the users Email</t>
+  </si>
+  <si>
+    <t>Can I Edit the users campus</t>
+  </si>
+  <si>
+    <t>Can I edit the users name</t>
+  </si>
+  <si>
+    <t>I should be able to change the type of user the user is</t>
+  </si>
+  <si>
+    <t>I should be able to update the users year</t>
+  </si>
+  <si>
+    <t>I should not be able to edit the users email</t>
+  </si>
+  <si>
+    <t>I should be able to edit the users campus</t>
+  </si>
+  <si>
+    <t>this did not work, this is because the value was gettting sent to the database, this was sending a string where it should be sending an int</t>
+  </si>
+  <si>
+    <t>This now works as intended</t>
+  </si>
+  <si>
+    <t>I should be able to edit the users name</t>
+  </si>
+  <si>
+    <t>this works as intended</t>
+  </si>
+  <si>
+    <t>can I remove a user</t>
+  </si>
+  <si>
+    <t>can I ban a user</t>
+  </si>
+  <si>
+    <t>pressing the remove user button should remove a user after a confimation box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pressing the ban user button should ban a user without removing them from the database </t>
+  </si>
+  <si>
+    <t>can a user book an item if they have been banned</t>
+  </si>
+  <si>
+    <t>if the user has been banned they should not be able to book an item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this works as intended as the user cannot get to any page on the website </t>
+  </si>
+  <si>
+    <t>when a user is banned can they accsess the website</t>
+  </si>
+  <si>
+    <t>they should not be able to accses any webpage on the site</t>
+  </si>
+  <si>
+    <t>can I unban a banned user</t>
+  </si>
+  <si>
+    <t>if a user has been banned they should be able to be unbanned by an admin</t>
+  </si>
+  <si>
+    <t>can a recently unbanned user accsess the website</t>
+  </si>
+  <si>
+    <t>if they have been unbanned they should be ablle to accsess the website as normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> this works as intended</t>
+  </si>
+  <si>
+    <t>Can the admin make a new owner</t>
+  </si>
+  <si>
+    <t>on the make/remove owner page they should be able to make new owners</t>
+  </si>
+  <si>
+    <t>this works as intended once they have filled in the form</t>
+  </si>
+  <si>
+    <t>can the admin remove someone as an owner</t>
+  </si>
+  <si>
+    <t>the admin should also be able to remove someone as an owner</t>
+  </si>
+  <si>
+    <t>this worked as intended</t>
+  </si>
+  <si>
+    <t>can the admin edit an owners infromation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user should also be able to edit an owners infromation </t>
+  </si>
+  <si>
+    <t>Can an owner see all of their inventory</t>
+  </si>
+  <si>
+    <t>can a owner edit their inventory</t>
+  </si>
+  <si>
+    <t>can an owner remove their inventory</t>
+  </si>
+  <si>
+    <t>can a user view the status of items that people want to book</t>
+  </si>
+  <si>
+    <t>can an owner confirm a booking</t>
+  </si>
+  <si>
+    <t>can an owner decline a bookin</t>
+  </si>
+  <si>
+    <t>can a owner select that the item has been returned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">can an owner view the types of agreements </t>
+  </si>
+  <si>
+    <t>can an owner view others agreements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">can an owner upload an agreement </t>
+  </si>
+  <si>
+    <t xml:space="preserve">can an staff member add an item if they have not been set to an owner </t>
+  </si>
+  <si>
+    <t xml:space="preserve">can an owner add an item </t>
+  </si>
+  <si>
+    <t>can an owner add a item name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">can an owner set an item agreement </t>
+  </si>
+  <si>
+    <t>can an owner set an item restiction</t>
+  </si>
+  <si>
+    <t>can an owner set if the item needs supervision</t>
+  </si>
+  <si>
+    <t>can an owner set the items condition</t>
+  </si>
+  <si>
+    <t>can an own upload an image</t>
+  </si>
+  <si>
+    <t>can the owner view the agrement they have choosen on the same page when they're adding an item</t>
+  </si>
+  <si>
+    <t>does the new item show in the catalogue</t>
+  </si>
+  <si>
+    <t>does the new items information show correclty</t>
+  </si>
+  <si>
+    <t>does the new item have the correct image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">does the item show under the correct type </t>
+  </si>
+  <si>
+    <t>can an owner change the type of their item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">when navagating to the my inventory page the owner should be able to view all of their current inventory </t>
+  </si>
+  <si>
+    <t>The user should be able to edit the information about their item, such as name and condiiton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this works as intended </t>
+  </si>
+  <si>
+    <t>the user should be able to remove their own inventory</t>
+  </si>
+  <si>
+    <t>the owner has to confirm a booking ,this allowing them to keep track of who is borrowing their items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if the owner accepts the booking condions they should be able to confirm the booking </t>
+  </si>
+  <si>
+    <t xml:space="preserve">if the owner does not accept the booking condions they should be able to deny the booking </t>
+  </si>
+  <si>
+    <t>if the item has been returned the owner should be able to say that they have recived the item back</t>
+  </si>
+  <si>
+    <t>the owner should be able to see the agreements on the system, this allowing them to choose which one they might want to user</t>
+  </si>
+  <si>
+    <t>the owner might want to view other peoples agreements that they might want to use themselves</t>
+  </si>
+  <si>
+    <t>on the page where they can upload an agreement they should be able to upload a txt file</t>
+  </si>
+  <si>
+    <t>if an staff member has not been set as an owner yet then they should not be able to upload an item</t>
+  </si>
+  <si>
+    <t>this works but not 100% the item does not get added but the image still uploads</t>
+  </si>
+  <si>
+    <t>if the staff has not been set as an owner yet then they shoould not have the navagation option, this can be fixed with an if statement on the php</t>
+  </si>
+  <si>
+    <t>if the staff has been set to an owner they should be able to upload a new item</t>
+  </si>
+  <si>
+    <t>the owner should be able to add an item name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the owner should be able to add an item type </t>
+  </si>
+  <si>
+    <t>can an owner add an item type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the owner should be able to select an item agreement </t>
+  </si>
+  <si>
+    <t>the owner should be able to set an item restiction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the owner should be able to set if they want the item to be supervised </t>
+  </si>
+  <si>
+    <t xml:space="preserve">the owner hsould be able to set the items condition </t>
+  </si>
+  <si>
+    <t>the owner should be able to add an item image</t>
+  </si>
+  <si>
+    <t>if the owner has selected an agreement they should be able to view the current agreement just in case they want to check it</t>
+  </si>
+  <si>
+    <t>the new item should appear in the catalogue</t>
+  </si>
+  <si>
+    <t>the item should be uploaded with the correct infromation</t>
+  </si>
+  <si>
+    <t>the image should be the one uploaded</t>
+  </si>
+  <si>
+    <t>the item should have the type that the user has choosen</t>
+  </si>
+  <si>
+    <t>if the user has pressed the wrong type they should be able to change it</t>
   </si>
 </sst>
 </file>
@@ -571,7 +982,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -596,6 +1007,9 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -920,138 +1334,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J76"/>
+  <dimension ref="A1:J137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD29"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="6.140625" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="6" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="2.28515625" customWidth="1"/>
+    <col min="7" max="7" width="65.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
+    <row r="1" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="H5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -1059,7 +1469,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -1067,556 +1477,556 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+      <c r="B11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="D11" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="D15" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
+      <c r="B19" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="D19" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>5</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>6</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>7</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>8</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>9</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="H24" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="4" t="s">
+    </row>
+    <row r="25" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>10</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="102" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
-        <v>10</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>70</v>
-      </c>
       <c r="E25" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>11</v>
       </c>
       <c r="B26" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H26" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="4" t="s">
+    </row>
+    <row r="27" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
+        <v>12</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A27" s="4">
-        <v>12</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="E27" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>13</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>14</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>81</v>
-      </c>
       <c r="E29" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
@@ -1624,198 +2034,198 @@
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
     </row>
-    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
     </row>
-    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>15</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>16</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>16</v>
       </c>
       <c r="B35" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G35" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="H35" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>17</v>
       </c>
       <c r="B36" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H36" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>18</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>19</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="114.75" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>20</v>
       </c>
       <c r="B39" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="H39" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
@@ -1823,25 +2233,25 @@
         <v>21</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
@@ -1849,25 +2259,25 @@
         <v>22</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -1880,61 +2290,60 @@
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
     </row>
+    <row r="43" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>110</v>
-      </c>
+      <c r="A44" s="1"/>
     </row>
     <row r="45" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>23</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>24</v>
       </c>
       <c r="B46" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D46" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>116</v>
-      </c>
       <c r="E46" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="H46" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
@@ -1942,51 +2351,51 @@
         <v>25</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>26</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -1994,25 +2403,25 @@
         <v>27</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="I49" s="11">
         <v>42754</v>
@@ -2023,25 +2432,25 @@
         <v>28</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -2049,25 +2458,25 @@
         <v>29</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -2075,25 +2484,25 @@
         <v>30</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -2101,25 +2510,25 @@
         <v>31</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -2127,51 +2536,51 @@
         <v>32</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>33</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -2179,78 +2588,118 @@
         <v>34</v>
       </c>
       <c r="B56" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D56" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C56" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>139</v>
-      </c>
       <c r="E56" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>35</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C57" s="6"/>
-      <c r="D57" s="6"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="6"/>
-      <c r="G57" s="6"/>
-      <c r="H57" s="6"/>
+        <v>135</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="H57" s="6" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="58" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>36</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="6"/>
-      <c r="G58" s="6"/>
-      <c r="H58" s="6"/>
+        <v>136</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H58" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="59" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <v>37</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C59" s="6"/>
-      <c r="D59" s="6"/>
-      <c r="E59" s="6"/>
-      <c r="F59" s="6"/>
-      <c r="G59" s="6"/>
-      <c r="H59" s="6"/>
+        <v>137</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H59" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="60" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>38</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C60" s="6"/>
-      <c r="D60" s="6"/>
+        <v>138</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>189</v>
+      </c>
       <c r="E60" s="6"/>
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
@@ -2261,10 +2710,14 @@
         <v>39</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C61" s="6"/>
-      <c r="D61" s="6"/>
+        <v>139</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>189</v>
+      </c>
       <c r="E61" s="6"/>
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
@@ -2275,24 +2728,36 @@
         <v>40</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C62" s="6"/>
-      <c r="D62" s="6"/>
-      <c r="E62" s="6"/>
-      <c r="F62" s="6"/>
+        <v>140</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>112</v>
+      </c>
       <c r="G62" s="6"/>
       <c r="H62" s="6"/>
     </row>
-    <row r="63" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
         <v>41</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C63" s="6"/>
-      <c r="D63" s="6"/>
+        <v>141</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>189</v>
+      </c>
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
@@ -2303,10 +2768,14 @@
         <v>42</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="C64" s="6"/>
-      <c r="D64" s="6"/>
+        <v>142</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>189</v>
+      </c>
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
@@ -2317,79 +2786,99 @@
         <v>43</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C65" s="6"/>
-      <c r="D65" s="6"/>
-      <c r="E65" s="6"/>
-      <c r="F65" s="6"/>
-      <c r="G65" s="6"/>
-      <c r="H65" s="6"/>
+        <v>143</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="H65" s="6" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="66" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
         <v>44</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C66" s="6"/>
-      <c r="D66" s="6"/>
-      <c r="E66" s="6"/>
-      <c r="F66" s="6"/>
+        <v>144</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>112</v>
+      </c>
       <c r="G66" s="6"/>
       <c r="H66" s="6"/>
     </row>
-    <row r="67" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
         <v>45</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
         <v>46</v>
       </c>
       <c r="B68" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D68" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C68" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>155</v>
-      </c>
       <c r="E68" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -2397,39 +2886,59 @@
         <v>47</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D69" s="6"/>
-      <c r="E69" s="6"/>
-      <c r="F69" s="6"/>
-      <c r="G69" s="6"/>
-      <c r="H69" s="6"/>
-    </row>
-    <row r="70" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G69" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="H69" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
         <v>48</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="D70" s="6"/>
-      <c r="E70" s="6"/>
-      <c r="F70" s="6"/>
-      <c r="G70" s="6"/>
-      <c r="H70" s="6"/>
+        <v>154</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H70" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="71" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="6">
         <v>49</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C71" s="6"/>
       <c r="D71" s="6"/>
@@ -2438,12 +2947,12 @@
       <c r="G71" s="6"/>
       <c r="H71" s="6"/>
     </row>
-    <row r="72" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A72" s="6">
         <v>50</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C72" s="6"/>
       <c r="D72" s="6"/>
@@ -2457,7 +2966,7 @@
         <v>51</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C73" s="6"/>
       <c r="D73" s="6"/>
@@ -2466,47 +2975,1471 @@
       <c r="G73" s="6"/>
       <c r="H73" s="6"/>
     </row>
-    <row r="74" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A74" s="6">
         <v>52</v>
       </c>
-      <c r="B74" s="6" t="s">
+      <c r="B74" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D74" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="C74" s="6"/>
-      <c r="D74" s="6"/>
-      <c r="E74" s="6"/>
-      <c r="F74" s="6"/>
-      <c r="G74" s="6"/>
-      <c r="H74" s="6"/>
-    </row>
-    <row r="75" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E74" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G74" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="H74" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A75" s="6">
         <v>53</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C75" s="6"/>
-      <c r="D75" s="6"/>
-      <c r="E75" s="6"/>
-      <c r="F75" s="6"/>
-      <c r="G75" s="6"/>
-      <c r="H75" s="6"/>
-    </row>
-    <row r="76" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="H75" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A76" s="6">
         <v>54</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C76" s="6"/>
+        <v>166</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>167</v>
+      </c>
       <c r="D76" s="6"/>
       <c r="E76" s="6"/>
       <c r="F76" s="6"/>
       <c r="G76" s="6"/>
       <c r="H76" s="6"/>
+    </row>
+    <row r="77" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A77" s="6">
+        <v>55</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H77" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A78" s="6">
+        <v>56</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G78" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H78" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A79" s="6">
+        <v>57</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H79" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A80" s="6">
+        <v>58</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H80" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A81" s="6">
+        <v>59</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G81" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="H81" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A82" s="6">
+        <v>60</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="G82" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="H82" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A83" s="6">
+        <v>61</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6"/>
+    </row>
+    <row r="84" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A84" s="6">
+        <v>62</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+    </row>
+    <row r="85" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A85" s="6">
+        <v>63</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
+    </row>
+    <row r="86" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A86" s="6">
+        <v>64</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="E86" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G86" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="H86" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A87" s="6">
+        <v>65</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G87" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H87" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A88" s="6">
+        <v>66</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E88" s="6"/>
+      <c r="F88" s="6"/>
+      <c r="G88" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H88" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A89" s="6">
+        <v>67</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E89" s="6"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H89" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A90" s="6">
+        <v>68</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H90" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A91" s="6">
+        <v>69</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D91" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="E91" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F91" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="G91" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="H91" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A92" s="6">
+        <v>70</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="E92" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F92" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G92" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H92" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A93" s="6">
+        <v>71</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E93" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F93" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G93" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H93" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A94" s="6">
+        <v>72</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="D94" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E94" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F94" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G94" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H94" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A95" s="6">
+        <v>73</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="D95" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E95" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F95" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G95" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H95" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A96" s="6">
+        <v>74</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="D96" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="E96" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F96" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G96" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H96" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A97" s="6">
+        <v>75</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="D97" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E97" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F97" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G97" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H97" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A98" s="6">
+        <v>76</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="D98" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E98" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F98" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G98" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H98" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A99" s="6">
+        <v>77</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="D99" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="E99" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F99" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G99" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H99" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A100" s="6">
+        <v>78</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="D100" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="E100" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F100" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G100" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H100" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A101" s="6">
+        <v>79</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="D101" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="E101" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F101" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G101" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H101" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A102" s="6">
+        <v>80</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="C102" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="D102" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E102" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F102" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G102" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H102" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A103" s="6">
+        <v>81</v>
+      </c>
+      <c r="B103" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="C103" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D103" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E103" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F103" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G103" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H103" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A104" s="6">
+        <v>82</v>
+      </c>
+      <c r="B104" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="C104" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="D104" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E104" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F104" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G104" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H104" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A105" s="6">
+        <v>83</v>
+      </c>
+      <c r="B105" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E105" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F105" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G105" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H105" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A106" s="6">
+        <v>84</v>
+      </c>
+      <c r="B106" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="C106" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="D106" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E106" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F106" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G106" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H106" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A107" s="6">
+        <v>85</v>
+      </c>
+      <c r="B107" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="C107" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="D107" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E107" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F107" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G107" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H107" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A108" s="6">
+        <v>86</v>
+      </c>
+      <c r="B108" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="C108" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="D108" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E108" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F108" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G108" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H108" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A109" s="6">
+        <v>87</v>
+      </c>
+      <c r="B109" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C109" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D109" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="E109" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F109" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G109" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H109" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A110" s="6">
+        <v>88</v>
+      </c>
+      <c r="B110" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="C110" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="D110" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E110" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F110" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G110" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H110" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A111" s="6">
+        <v>89</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="C111" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E111" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F111" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G111" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H111" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A112" s="6">
+        <v>90</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="C112" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="D112" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E112" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F112" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G112" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H112" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A113" s="6">
+        <v>91</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="E113" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F113" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="G113" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="H113" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A114" s="6">
+        <v>92</v>
+      </c>
+      <c r="B114" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="C114" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="D114" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E114" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F114" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G114" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H114" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A115" s="6">
+        <v>93</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="C115" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="D115" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E115" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F115" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G115" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H115" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A116" s="6">
+        <v>94</v>
+      </c>
+      <c r="B116" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="C116" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="D116" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E116" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F116" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G116" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H116" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A117" s="6">
+        <v>95</v>
+      </c>
+      <c r="B117" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="C117" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="D117" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E117" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F117" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G117" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H117" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A118" s="6">
+        <v>96</v>
+      </c>
+      <c r="B118" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="D118" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E118" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F118" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G118" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H118" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A119" s="6">
+        <v>97</v>
+      </c>
+      <c r="B119" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="C119" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="D119" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E119" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F119" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G119" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H119" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A120" s="6">
+        <v>98</v>
+      </c>
+      <c r="B120" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="C120" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="D120" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E120" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F120" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G120" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H120" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A121" s="6">
+        <v>99</v>
+      </c>
+      <c r="B121" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="C121" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="D121" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E121" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F121" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G121" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H121" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A122" s="6">
+        <v>100</v>
+      </c>
+      <c r="B122" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="C122" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="D122" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E122" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F122" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G122" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H122" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A123" s="6">
+        <v>101</v>
+      </c>
+      <c r="B123" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="C123" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="D123" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E123" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F123" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G123" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H123" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A124" s="6">
+        <v>102</v>
+      </c>
+      <c r="B124" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="C124" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="D124" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E124" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F124" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G124" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H124" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A125" s="6">
+        <v>103</v>
+      </c>
+      <c r="B125" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="C125" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="D125" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E125" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F125" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G125" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H125" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A126" s="6">
+        <v>104</v>
+      </c>
+      <c r="B126" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="C126" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="D126" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E126" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F126" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G126" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H126" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A127" s="6">
+        <v>105</v>
+      </c>
+      <c r="B127" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="C127" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="D127" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E127" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F127" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G127" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H127" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A128" s="6">
+        <v>106</v>
+      </c>
+      <c r="B128" s="6"/>
+      <c r="C128" s="6"/>
+      <c r="D128" s="6"/>
+      <c r="E128" s="6"/>
+      <c r="F128" s="6"/>
+      <c r="G128" s="6"/>
+      <c r="H128" s="6"/>
+    </row>
+    <row r="129" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A129" s="6">
+        <v>107</v>
+      </c>
+      <c r="B129" s="6"/>
+      <c r="C129" s="6"/>
+      <c r="D129" s="6"/>
+      <c r="E129" s="6"/>
+      <c r="F129" s="6"/>
+      <c r="G129" s="6"/>
+      <c r="H129" s="6"/>
+    </row>
+    <row r="130" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A130" s="6">
+        <v>108</v>
+      </c>
+      <c r="B130" s="6"/>
+      <c r="C130" s="6"/>
+      <c r="D130" s="6"/>
+      <c r="E130" s="6"/>
+      <c r="F130" s="6"/>
+      <c r="G130" s="6"/>
+      <c r="H130" s="6"/>
+    </row>
+    <row r="131" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A131" s="6">
+        <v>109</v>
+      </c>
+      <c r="B131" s="6"/>
+      <c r="C131" s="6"/>
+      <c r="D131" s="6"/>
+      <c r="E131" s="6"/>
+      <c r="F131" s="6"/>
+      <c r="G131" s="6"/>
+      <c r="H131" s="6"/>
+    </row>
+    <row r="132" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A132" s="6">
+        <v>110</v>
+      </c>
+      <c r="B132" s="6"/>
+      <c r="C132" s="6"/>
+      <c r="D132" s="6"/>
+      <c r="E132" s="6"/>
+      <c r="F132" s="6"/>
+      <c r="G132" s="6"/>
+      <c r="H132" s="6"/>
+    </row>
+    <row r="133" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A133" s="6">
+        <v>111</v>
+      </c>
+      <c r="B133" s="6"/>
+      <c r="C133" s="6"/>
+      <c r="D133" s="6"/>
+      <c r="E133" s="6"/>
+      <c r="F133" s="6"/>
+      <c r="G133" s="6"/>
+      <c r="H133" s="6"/>
+    </row>
+    <row r="134" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A134" s="6">
+        <v>112</v>
+      </c>
+      <c r="B134" s="6"/>
+      <c r="C134" s="6"/>
+      <c r="D134" s="6"/>
+      <c r="E134" s="6"/>
+      <c r="F134" s="6"/>
+      <c r="G134" s="6"/>
+      <c r="H134" s="6"/>
+    </row>
+    <row r="135" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A135" s="6">
+        <v>113</v>
+      </c>
+      <c r="B135" s="6"/>
+      <c r="C135" s="6"/>
+      <c r="D135" s="6"/>
+      <c r="E135" s="6"/>
+      <c r="F135" s="6"/>
+      <c r="G135" s="6"/>
+      <c r="H135" s="6"/>
+    </row>
+    <row r="136" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A136" s="6">
+        <v>114</v>
+      </c>
+      <c r="B136" s="6"/>
+      <c r="C136" s="6"/>
+      <c r="D136" s="6"/>
+      <c r="E136" s="6"/>
+      <c r="F136" s="6"/>
+      <c r="G136" s="6"/>
+      <c r="H136" s="6"/>
+    </row>
+    <row r="137" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A137" s="6">
+        <v>115</v>
+      </c>
+      <c r="B137" s="6"/>
+      <c r="C137" s="6"/>
+      <c r="D137" s="6"/>
+      <c r="E137" s="6"/>
+      <c r="F137" s="6"/>
+      <c r="G137" s="6"/>
+      <c r="H137" s="6"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L9">

</xml_diff>